<commit_message>
Many updates to Code - have not pushed changes for a while
Pushing changes including updating with new metrics
</commit_message>
<xml_diff>
--- a/Data/Habitat_Data/Barriers_Pathway_Data.xlsx
+++ b/Data/Habitat_Data/Barriers_Pathway_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Habitat_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF8BB83-76B5-4B9E-ACA0-F72E5DB35041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455693E4-3B90-463E-AAEB-DB1AE2D1293B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3012" yWindow="1524" windowWidth="20172" windowHeight="11544" xr2:uid="{DB42646B-B34B-48E8-9287-DB4643A7764E}"/>
+    <workbookView xWindow="1380" yWindow="1695" windowWidth="24900" windowHeight="13020" xr2:uid="{DB42646B-B34B-48E8-9287-DB4643A7764E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>ReachName</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>Wenatchee</t>
-  </si>
-  <si>
-    <t>Big Meadow Creek</t>
-  </si>
-  <si>
-    <t>Big Meadow Creek 01</t>
   </si>
   <si>
     <t>Lower Icicle Creek</t>
@@ -218,9 +212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,7 +252,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -364,7 +358,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -506,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,25 +508,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B127C54-B5A6-4ECF-8558-DF4840F07D29}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -544,10 +539,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -564,10 +559,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -584,10 +579,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -604,18 +599,18 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>6</v>
@@ -624,27 +619,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>